<commit_message>
feat : missions.xlsx 파일 수정 - #15
</commit_message>
<xml_diff>
--- a/src/main/resources/data/missions.xlsx
+++ b/src/main/resources/data/missions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaahyeonseo/Desktop/Spring/Bjjm/src/main/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{54CE943E-898F-3746-BECB-B37B583BC6C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F22F6862-0FFD-334D-B669-CC09BC5BD3B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="760" windowWidth="22740" windowHeight="17060" xr2:uid="{FEC315C9-F979-074A-BA3E-305C2FA7C52A}"/>
+    <workbookView xWindow="640" yWindow="760" windowWidth="18700" windowHeight="16980" xr2:uid="{FEC315C9-F979-074A-BA3E-305C2FA7C52A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>region</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -63,6 +63,61 @@
   </si>
   <si>
     <t>y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>해운대 해수욕장 인증샷</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>동백섬 산책</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자갈치 시장 구경</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>바다와 함께 인증샷 찍기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>동백섬 트래킹하기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시장 속 활기 느끼기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>해운대 해수욕장에서 셀카나 풍경사진을 찍으세요!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>동백섬 코스를 따라 걸으며 사진을 남겨보세요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자갈치 시장에서 인증샷과 함께 부산의 전통을 즐겨보세요.</t>
+  </si>
+  <si>
+    <t>https://example.com/haeundae1.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://example.com/dongbaek.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://example.com/jagalchi.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>해운대구</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>중구</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -70,7 +125,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -81,6 +136,20 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF6AAB73"/>
+      <name val="Menlo-Regular"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
@@ -104,18 +173,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="하이퍼링크" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -447,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11CF1E01-9D5A-7D45-A709-4330EE0430DB}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -478,8 +557,88 @@
         <v>6</v>
       </c>
     </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2">
+        <v>129.15799999999999</v>
+      </c>
+      <c r="G2">
+        <v>35.162999999999997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3">
+        <v>129.15299999999999</v>
+      </c>
+      <c r="G3">
+        <v>35.156999999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4">
+        <v>129.03700000000001</v>
+      </c>
+      <c r="G4">
+        <v>35.097000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="D5" s="1"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="D8" s="2"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{BCFE28CC-7740-0E48-B166-98FD876221D7}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{D6EC605C-67D7-A941-A13A-5E3AE0691E27}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{1D2D18DA-A1A9-A943-B389-C4A1BA1FAADC}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat : missions.xlsx 내용 수정 - #21
</commit_message>
<xml_diff>
--- a/src/main/resources/data/missions.xlsx
+++ b/src/main/resources/data/missions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaahyeonseo/Desktop/Spring/Bjjm/src/main/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F22F6862-0FFD-334D-B669-CC09BC5BD3B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{215FBBCB-5AAD-744D-AD77-D4052282446E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="640" yWindow="760" windowWidth="18700" windowHeight="16980" xr2:uid="{FEC315C9-F979-074A-BA3E-305C2FA7C52A}"/>
   </bookViews>
@@ -38,34 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
-    <t>region</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>title</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>introduction</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>content</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>imageUrl</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>x</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>y</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>해운대 해수욕장 인증샷</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -118,6 +90,34 @@
   </si>
   <si>
     <t>중구</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x(경도)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y(위도)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>imageUrl(미션 이미지)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>introduction(미션 한 줄 소개부분이에요!)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>title(미션제목)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>region(미션 지역 : 수영구, 해운대구, 금정구, 동래구, 중구, 동구, 기장군, 사하구, 사상구, 영도구, 강서구, 부산진구, 서구, 남구, 북구, 연제구)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>content(미션 내용: 줄바꿈 필요할 시에 &lt;/br&gt;로 줄바꿈 표시해주세요!)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -529,49 +529,49 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="F2">
         <v>129.15799999999999</v>
@@ -582,19 +582,19 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F3">
         <v>129.15299999999999</v>
@@ -605,19 +605,19 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="F4">
         <v>129.03700000000001</v>

</xml_diff>

<commit_message>
file : missions.xlsx 최종 수정
</commit_message>
<xml_diff>
--- a/src/main/resources/data/missions.xlsx
+++ b/src/main/resources/data/missions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaahyeonseo/Desktop/Spring/Bjjm/src/main/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D3274BA-70E4-AC45-850C-116E1CD8EAE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21AE0E7E-539F-754E-B1F3-579C81CAA504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="920" windowWidth="29080" windowHeight="13560" xr2:uid="{FEC315C9-F979-074A-BA3E-305C2FA7C52A}"/>
+    <workbookView xWindow="160" yWindow="920" windowWidth="29080" windowHeight="16620" xr2:uid="{FEC315C9-F979-074A-BA3E-305C2FA7C52A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1137,469 +1137,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1️⃣ 수영구의 매력을 느끼며 관광을 시작해보세요.\n2️⃣ 해변 요가, 서핑, 패들 보드 등 다양한 해양레포츠를 미리 예약해 준비하세요.\n📌 예약 링크 :http://www.crazy-surfers.com \n3️⃣ 광안리 SUP ZONE에 도착해 위치 인증을 남겨보세요.\n4️⃣ SUP ZONE에서 레포츠를 즐기며 사진과 함께 생생한 후기를 기록하세요.\n</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1️⃣ 수영구 명소를 둘러보며 저녁 시간을 준비하세요. \n2️⃣ 매주 토요일, 광안리 해변에서 열리는 드론 라이트쇼 시간을 확인하세요. \n- 하절기(3~9월) : 20시 / 22시 \n- 동절기(10~2월) : 19시 / 21시\n💡 기상이나 현장 상황에 따라 취소·지연될 수 있음.\n📌 안내 : [광안리 M 드론라이트쇼](https://www.gwangallimdrone.co.kr/)\n3️⃣ 광안리 해변에 도착해 위치 인증샷을 남겨보세요.\n4️⃣ 드론 라이트쇼의 화려한 순간을 사진으로 담고, 감상 후기를 작성하세요.\n</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1️⃣ </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>수영구 일대를 산책하며 분위기를 즐기세요.\n2️⃣ 2호선 남천역 2번 출구에서 내려 오르막길을 따라 도모헌까지 걸어가 보세요.\n3️⃣ 도모헌 입구에서 인증샷으로 방문을 기록하세요.\n
-4️⃣ 전시와 건물 곳곳을 관람하며, 인상 깊었던 장면을 사진과 후기로 남기세요.\n</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1️⃣ 수영구에서의 하루를 계획하며 관광을 시작하세요.\n2️⃣ 3호선 망미역 4번 출구에서 하차해 F1963까지 이동하세요.\n3️⃣ F1963 건물 앞에서 위치 인증샷을 남기세요.\n4️⃣ 과거 고려제강 와이어공장이었던 공간을 새롭게 재탄생시킨 문화명소를 둘러보세요.\n- 천장이 그대로 보존된 테라로사 커피숍\n- 감각적인 도서관\n- 다양한 전시와 문화 프로그램\n모든 경험을 사진과 후기로 기록하세요.\n</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1️⃣ 해운대구의 매력을 느끼며 관광을 시작하세요.\n2️⃣ [해운대 블루라인파크](https://www.bluelinepark.com/)에서 스카이캡슐 또는 해변열차를 예약하세요.\n3️⃣ 해변 구간을 달리며 옛 해안 절경을 감상하고, 위치 인증샷을 남기세요.\n4️⃣ 탑승 중 또는 도착지에서 찍은 멋진 풍경 사진과 체험 후기를 기록하세요.\n</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1️⃣ 해운대구를 거닐며 여행 분위기를 즐기세요.\n2️⃣ [부산 요트투어 예약 링크](https://search.shopping.naver.com/search/all?query=%ED%95%B4%EC%9A%B4%EB%8C%80%20%EC%9A%94%ED%8A%B8%20%ED%88%AC%EC%96%B4&amp;frm=NVSCPRO&amp;nl-ts-pid=j4AErdqo1awsshZRDwGssssst1V-348234&amp;bt=-1)를 통해 원하는 시간과 코스를 선택하세요.\n3️⃣ 요트에 승선해 바다 위에서의 특별한 순간을 즐기고 인증샷을 남기세요.\n4️⃣ 바다 풍경과 함께 담은 인생샷과 체험 후기를 작성하세요.\n</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1️⃣ 해운대구 명소를 둘러보며 영화 관람 계획을 세우세요.\n2️⃣ 2호선 센텀시티역 12번 출구에서 하차해 영화의전당으로 이동하세요.\n3️⃣ [영화의전당 예매 페이지](https://mobile.dureraum.org:44500/bccm/main/main.do?rbsIdx=1)에서 원하는 영화를 예약하거나, 더 라이브러리에서 무료 영화를 감상하세요.\n4️⃣ 영화 관람 후 건물 외관이나 야경을 배경으로 인증샷을 찍고 후기를 남기세요.\n</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1️⃣ 금정구 일대를 둘러보며 문학과 역사 여행을 준비하세요.\n2️⃣ [요산 김정한 문학관](https://sayosan.or.kr/)을 찾아가 입구에서 첫 인증샷을 남기세요.\n3️⃣ 김정한 작가의 생애와 작품 세계를 전시 자료와 함께 감상하세요.\n4️⃣ 기억에 남는 전시물이나 글귀를 사진과 후기 형식으로 기록하세요</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1️⃣ 금정구의 대표 사찰인 범어사를 목적지로 정하세요.\n2️⃣ 범어사 일주문을 지나 경내로 걸어 들어가며 고즈넉한 분위기를 느껴보세요.\n3️⃣ 대웅전, 범종각 등 주요 건물 앞에서 인증샷을 남기세요.\n4️⃣ 사찰의 풍경과 느낀 점을 후기에 담아 기록하세요.</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1️⃣ 금정산 자락에 위치한 금정산성 코스를 계획하세요.\n2️⃣ 등산로 또는 탐방로를 따라 금정산성에 도착하세요.\n3️⃣ 산성의 성문, 성벽 등 역사적인 포인트에서 인증샷을 남기세요.\n4️⃣ 산성과 금정구 전경을 함께 담은 사진과 함께 소감을 적어보세요.\n</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1️⃣ 동래구를 거닐며 옛 부산의 역사와 문화를 느껴보세요.\n2️⃣ 동래읍성 입구나 주요 성문(북문, 남문 등)에서 위치 인증샷을 찍으세요.\n3️⃣ 성벽을 따라 걸으며 조선 시대 방어 시설과 주변 경관을 감상하세요.\n4️⃣ 역사적인 배경과 함께 느낀 점을 후기에 기록하세요.\n</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1️⃣ 온천천을 따라 이어진 카페거리를 걸으며 여유로운 시간을 보내세요.\n2️⃣ 강변 산책로에서 계절별 풍경을 배경으로 인증샷을 남기세요.\n3️⃣ 마음에 드는 카페에 들러 음료를 즐기고 사진을 찍으세요.\n4️⃣ 온천천과 카페거리의 매력을 후기에 담으세요.\n</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1️⃣ 동래구의 전통 온천 문화를 체험할 계획을 세우세요.\n2️⃣ 온천탕이나 스파 시설에 방문해 위치 인증샷을 남기세요.\n3️⃣ 따뜻한 온천물에 몸을 담그며 피로를 풀어보세요.\n4️⃣ 온천 후 상쾌해진 기분과 추천 포인트를 후기에 작성하세요.\n</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1️⃣ 금강공원 입구로 이동해 케이블카 탑승 준비를 하세요.\n2️⃣ 케이블카 승강장에서 위치 인증샷을 찍으세요.\n3️⃣ 케이블카를 타고 금정산과 부산 시내 전망을 감상하세요.\n4️⃣ 정상에서 바라본 경치와 케이블카 경험을 후기에 기록하세요.\n</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1️⃣ 중구로 이동해 독립·예술 영화의 매력을 느껴보세요.\n2️⃣ BNK부산은행 아트시네마 또는 모퉁이극장 입구에서 위치 인증샷을 찍으세요.\n3️⃣ 상영작을 관람하며 영화 속 몰입감을 즐기세요.\n4️⃣ 영화 감상 후 인상 깊었던 장면과 분위기를 후기에 기록하세요.\n</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1️⃣ 보수동 골목길로 들어서며 중구의 문화 향기를 느껴보세요.\n2️⃣ 오래된 헌책방 간판과 골목 풍경을 배경으로 위치 인증샷을 남기세요.\n3️⃣ 마음에 드는 책을 한 권 골라 구입하거나 읽어보세요.\n4️⃣ 책방골목에서 느낀 레트로 감성과 발견한 책 이야기를 후기에 작성하세요.\n</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1️⃣ </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>대청동 일대에 위치한 전망대로 이동하세요.\n2️⃣ 전망대 입구나 내부에서 위치 인증샷을 남기세요.\n3️⃣ 부산항과 남포동 일대가 한눈에 보이는 전망을 감상하세요.\n4️⃣ 탁 트인 경치와 촬영한 사진을 후기에 기록하세요.\n</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1️⃣ 아미동 골목길을 따라 비석마을로 향하세요.\n2️⃣ 마을 입구나 벽화 앞에서 위치 인증샷을 찍으세요.\n3️⃣ 독특한 역사와 사연이 깃든 마을을 천천히 걸으며 둘러보세요.\n4️⃣ 마을의 분위기와 인상 깊었던 포인트를 후기에 남기세요.\n</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1️⃣ 중구 광복동에 있는 부산근현대역사관으로 이동하세요.\n2️⃣ 역사관 입구에서 위치 인증샷을 남기세요.\n3️⃣ 전시실을 둘러보며 부산의 근현대사를 배우세요.\n4️⃣ 인상 깊었던 전시 내용과 느낀 점을 후기에 성하세요.\n</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1️⃣ 용두산공원으로 이동해 부산타워로 향하세요.\n2️⃣ 타워 입구나 전망대에서 위치 인증샷을 남기세요.\n3️⃣ 부산 시내 전경과 바다를 한눈에 내려다보며 감상하세요.\n4️⃣ 찍은 사진과 함께 전망대에서의 경험을 후기에 남기세요.\n</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1️⃣ 동구로 이동해 창비부산 서점·문화공간을 방문하세요.\n2️⃣ 입구 간판이나 내부 전경에서 위치 인증샷을 남기세요.\n3️⃣ 책을 둘러보고, 마음에 드는 책을 골라 읽거나 구입하세요.\n4️⃣ 책과 함께한 시간, 공간 분위기를 후기에 기록하세요.\n</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1️⃣ 초량이바구길 시작 지점으로 이동하세요.\n2️⃣ 초량전망대나 벽화 앞에서 위치 인증샷을 찍으세요.\n3️⃣ 길을 따라 부산항과 시내 전경을 감상하며 걸어보세요.\n4️⃣ 산책 중 인상 깊었던 포인트와 사진을 후기에 남기세요.\n</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1️⃣ 부산역 인근 차이나타운 입구로 이동하세요.\n2️⃣ 붉은 아치형 간판이나 랜드마크 앞에서 위치 인증샷을 남기세요.\n3️⃣ 중국풍 음식점, 상점, 거리 예술을 구경하며 즐기세요.\n4️⃣ 먹은 음식과 거리 풍경 사진을 후기에 작성하세요.\n</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1️⃣ 168계단 인근에 위치한 야외영화관으로 이동하세요.\n2️⃣ 영화관 전경 또는 좌석에서 위치 인증샷을 남기세요.\n3️⃣ 야외에서 상영되는 영화를 감상하세요.\n4️⃣ 관람한 영화와 야외 분위기를 후기에 남기세요.\n</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1️⃣ 한복 문화관으로 이동해 전통 의상을 체험하세요.\n2️⃣ 입구 또는 한복 착용 후 위치 인증샷을 찍으세요.\n3️⃣ 전통 의상과 소품을 활용해 사진 촬영을 즐기세요.\n4️⃣ 체험 후 느낀 소감과 사진을 후기에 기록하세요.\n</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1️⃣ 기장군 해안 절벽 위의 해동용궁사로 이동하세요.\n2️⃣ 사찰 입구나 해안 풍경 앞에서 위치 인증샷을 남기세요.\n3️⃣ 사찰 내부와 주변 경관을 둘러보며 사진 촬영하세요.\n4️⃣ 해안 절경과 사찰의 매력을 후기에 작성하세요\n</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1️⃣ 테마파크 입구로 이동하세요.\n2️⃣ 롯데월드 조형물 앞에서 위치 인증샷을 남기세요.\n3️⃣ 놀이기구, 퍼레이드, 공연 등을 즐기세요.\n4️⃣ 가장 즐거웠던 순간과 사진을 후기에 기록하세요.\n</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1️⃣ 루지 체험장 입구로 이동하세요.\n2️⃣ 헬멧 착용 후 시작 지점에서 위치 인증샷을 남기세요.\n3️⃣ 루지 트랙을 내려가며 짜릿한 속도를 즐기세요.\n4️⃣ 체험 후 소감과 함께 사진을 후기에 남기세요.\n</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1️⃣ 연화리 해녀촌으로 이동하세요.\n2️⃣ 해녀촌 간판이나 바다 풍경 앞에서 위치 인증샷을 남기세요.\n3️⃣ 싱싱한 해산물 요리를 맛보세요.\n4️⃣ 맛본 음식과 바닷가 풍경을 후기에 작성하세요.\n</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1️⃣ 아홉산숲 입구로 이동하세요.\n2️⃣ 숲길 표지판이나 대나무 숲 앞에서 위치 인증샷을 남기세요.\n3️⃣ 대나무숲과 산책로를 따라 걸으며 자연을 느껴보세요.\n4️⃣ 숲에서의 힐링 경험과 사진을 후기에 기록하세요.\n</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1️⃣ 사하구 감천문화마을 입구로 이동하세요.\n2️⃣ 마을 입구 조형물이나 지도 앞에서 위치 인증샷을 남기세요.\n3️⃣ 골목길을 걸으며 벽화, 설치미술, 전망 포인트를 둘러보세요.\n4️⃣ 가장 마음에 드는 작품이나 풍경을 사진과 함께 후기에 기록하세요.\n</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1️⃣ 사하구 낙동강 하구에 위치한 부산현대미술관으로 이동하세요.\n2️⃣ 미술관 전경이나 전시 안내판 앞에서 위치 인증샷을 남기세요.\n3️⃣ 현재 진행 중인 전시를 관람하며 작품을 감상하세요.\n4️⃣ 인상 깊었던 작품과 느낀 점을 후기에 작성하세요.\n</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1️⃣ 을숙도 생태공원 입구로 이동하세요.\n2️⃣ 공원 표지판이나 전망대에서 위치 인증샷을 남기세요.\n3️⃣ 습지, 갈대밭, 철새 서식지를 둘러보며 산책하세요.\n4️⃣ 관찰한 풍경과 자연 속 경험을 후기에 기록하세요.\n</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1️⃣ 다대포해수욕장으로 이동하세요.\n2️⃣ 해변 안내판이나 백사장 앞에서 위치 인증샷을 남기세요.\n3️⃣ 바닷가를 산책하거나 노을 감상을 즐기세요.\n4️⃣ 노을 사진과 해변에서의 추억을 후기에 남기세요.\n</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>사상구</t>
   </si>
   <si>
@@ -1629,6 +1166,10 @@
     <t>자연과 강을 품은 부산 최대 규모 생태공원</t>
   </si>
   <si>
+    <t>https://www.visitbusan.net/uploadImgs/files/cntnts/20230602100722403</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="12"/>
@@ -1636,7 +1177,956 @@
         <rFont val="Segoe UI Emoji"/>
         <family val="2"/>
       </rPr>
-      <t>1️⃣</t>
+      <t>🏺</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 사상생활사박물관 관람</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>옛 사상 지역의 생활과 역사를 엿볼 수 있는 공간</t>
+  </si>
+  <si>
+    <t>https://www.busan.go.kr/ImagePrint.do?dir=smartEditor&amp;savename=71426cee1ce844d4a9a54895f4457666&amp;realname=IMG_8531.JPG&amp;fileext=jpg&amp;filetype=image/jpeg&amp;filesize=125431</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영도구</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🪂</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 태종대 집라인 체험</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>바다 절벽 위 짜릿한 레저 스포츠</t>
+  </si>
+  <si>
+    <t>https://www.visitbusan.net/uploadImgs/files/cntnts/20240718110728540</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>🏘</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 흰여울문화마을 산책</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>바다와 맞닿은 흰 담장 골목 예술마을</t>
+  </si>
+  <si>
+    <t>https://www.agoda.com/wp-content/uploads/2024/08/Huinnyeoul-Culture-Village-Busan-featured-1244x700.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>🖼</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 아르떼뮤지엄 부산 탐방</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몰입형 미디어아트 전시관</t>
+  </si>
+  <si>
+    <t>https://www.visitbusan.net/uploadImgs/files/cntnts/20240912162614628_oen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>강서구</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🌿</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 맥도생태공원 산책</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>도심 속 습지와 철새를 만날 수 있는 생태공원</t>
+  </si>
+  <si>
+    <t>https://media.triple.guide/triple-cms/c_limit,f_auto,h_1024,w_1024/94526eee-db87-4a21-86be-fa8f037db618.jpeg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부산진구</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🌳</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 부산시민공원 산책</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>도심 속에서 즐기는 여유로운 녹지 공간</t>
+  </si>
+  <si>
+    <t>https://www.visitbusan.net/uploadImgs/files/cntnts/20191227194943122_oen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>☕</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 전포 카페거리 투어</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>감각적인 카페와 맛집이 모인 핫플레이스</t>
+  </si>
+  <si>
+    <t>https://www.visitbusan.net/uploadImgs/files/cntnts/20191227195612923</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🌄</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 황령산 봉수대 전망</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부산 야경을 한눈에 즐기는 명소</t>
+  </si>
+  <si>
+    <t>https://mblogthumb-phinf.pstatic.net/MjAyMDAyMTNfMTAg/MDAxNTgxNTYwNjQ3NDcx.Qx1iMfelSbQjsjrwHRiSir-5cYl6twb3YLaWSMd2kdQg.KfALGkJ_wnbuqg4L1JEzclP7L6hRY_qJlDY7Sr78W0Mg.JPEG.springlll8/1.JPG?type=w800</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🎶</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 국립부산국악원 관람</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>우리 소리를 만나는 국악 전용 공연장</t>
+  </si>
+  <si>
+    <t>https://www.visitbusan.net/uploadImgs/files/cntnts/20240822173844772_oen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🛕</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 삼광사 탐방</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>화려한 연등으로 유명한 사찰</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcTOwlmY8_U_7f1NUP_n3MGoJiqYq5X8ZrFLPg&amp;s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>🛍</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 부전시장 탐방</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부산 대표 전통시장 중 하나</t>
+  </si>
+  <si>
+    <t>https://www.visitbusan.net/uploadImgs/files/cntnts/20191227113458027_oen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서구</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>🏖</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 송도해수욕장 즐기기</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대한민국 최초의 해수욕장</t>
+  </si>
+  <si>
+    <t>https://www.visitbusan.net/uploadImgs/files/cntnts/20191225175459392</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🚡</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 송도해상케이블카 탑승</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>송도 바다 위를 나는 케이블카</t>
+  </si>
+  <si>
+    <t>https://www.visitbusan.net/uploadImgs/files/cntnts/20230508183214812</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🎨</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 아미 비석문화마을 산책</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>예술과 역사가 공존하는 벽화 마을</t>
+  </si>
+  <si>
+    <t>https://www.visitbusan.net/uploadImgs/files/cntnts/20191226093556574_oen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🌲</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 암남공원 탐방</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>천혜의 자연을 간직한 도심 속 공원</t>
+  </si>
+  <si>
+    <t>https://www.visitbusan.net/uploadImgs/files/cntnts/20191227112720208_oen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>🏛</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 임시수도기념관 관람</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>한국전쟁 당시 임시수도의 역사를 담은 공간</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcTyyao3EwU852Gs2a3-fpH2mu4D74a8WhliGQ&amp;s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>남구</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>🕊</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 유엔평화기념관 방문</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전쟁과 평화를 기억하는 국제적 공간</t>
+  </si>
+  <si>
+    <t>https://mblogthumb-phinf.pstatic.net/MjAyNDA3MjRfNTMg/MDAxNzIxODAxMTE3Mjg4.Lw9UAUpgllbjysF742wVLtx8qtjExbd2MGsFIDfBCbgg.2o8cJbl0EEKd5qSaam1laNOSRbnyfoAoLFr2S1Hlb90g.JPEG/%EC%82%AC%EC%A7%846.jpg?type=w800</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🏺</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 부산박물관 관람</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부산의 역사와 문화를 한눈에 볼 수 있는 곳</t>
+  </si>
+  <si>
+    <t>https://museum.busan.go.kr/humanframe/theme/museum_busan_2025/assets/img/content/exhibitorigin0001.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🌊</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 이기대 해안산책</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>해안 절경과 트레킹 코스를 즐길 수 있는 명소</t>
+  </si>
+  <si>
+    <t>https://i.namu.wiki/i/pLygk_uCGnTjhllty4djNljfJWcAqwt9zi-bIl4AE_xfZe764Z0D9iSw9aYWuauMlSxOQxuptAecnvEDoLB1wg.webp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>북구</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🌿</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 화명생태공원 탐방</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>강과 숲이 어우러진 생태체험 공간</t>
+  </si>
+  <si>
+    <t>https://localsegye.co.kr/news/data/2025/03/07/p1065569622910044_923_thum.JPG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🌹</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 화명장미공원 감상</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>화려한 장미가 만개하는 힐링 명소</t>
+  </si>
+  <si>
+    <t>https://www.visitbusan.net/uploadImgs/files/cntnts/20230519190619574</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>🛍</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 구포시장 탐방</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>북구 대표 전통시장</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcTCIlXoYpHO16msUWEyjdmN_ZWyda2HjNpurH6EPX5IaPHe7MWaF7scT2u5JzHJwZ3Vr5w&amp;usqp=CAU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>연제구</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🛕</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 마하사 탐방</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>연제구의 고즈넉한 사찰</t>
+  </si>
+  <si>
+    <t>https://www.visitbusan.net/uploadImgs/files/cntnts/20240911101725976</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🏺</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 연산동 고분군 관람</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>가야시대 고분 유적지 탐방</t>
+  </si>
+  <si>
+    <t>https://i.namu.wiki/i/ehwWOBrnbUCrjhJJ2Qsyukxmr6NppuZqVAYlyLrgAKhIiYhRiHthdO28IY7m6DXms6CmzF_h7lK-UDbFleJpxw.webp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>수영구의 매력을 느끼며 관광을 시작해보세요.\n해변 요가, 서핑, 패들 보드 등 다양한 해양레포츠를 미리 예약해 준비하세요.\n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>📌</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 예약 링크 :http://www.crazy-surfers.com \n광안리 SUP ZONE에 도착해 위치 인증을 남겨보세요.\nSUP ZONE에서 레포츠를 즐기며 사진과 함께 생생한 후기를 기록하세요.\n</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>수영구 명소를 둘러보며 저녁 시간을 준비하세요. \n매주 토요일, 광안리 해변에서 열리는 드론 라이트쇼 시간을 확인하세요. \n- 하절기(3~9월) : 20시 / 22시 \n- 동절기(10~2월) : 19시 / 21시\n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>💡</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 기상이나 현장 상황에 따라 취소·지연될 수 있음.\n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>📌</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 안내 : [광안리 M 드론라이트쇼](https://www.gwangallimdrone.co.kr/)\n광안리 해변에 도착해 위치 인증샷을 남겨보세요.\n드론 라이트쇼의 화려한 순간을 사진으로 담고, 감상 후기를 작성하세요.\n</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>수영구 일대를 산책하며 분위기를 즐기세요.\n2호선 남천역 2번 출구에서 내려 오르막길을 따라 도모헌까지 걸어가 보세요.\n도모헌 입구에서 인증샷으로 방문을 기록하세요.\n
+전시와 건물 곳곳을 관람하며, 인상 깊었던 장면을 사진과 후기로 남기세요.\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>수영구에서의 하루를 계획하며 관광을 시작하세요.\n3호선 망미역 4번 출구에서 하차해 F1963까지 이동하세요.\nF1963 건물 앞에서 위치 인증샷을 남기세요.\n과거 고려제강 와이어공장이었던 공간을 새롭게 재탄생시킨 문화명소를 둘러보세요.\n- 천장이 그대로 보존된 테라로사 커피숍\n- 감각적인 도서관\n- 다양한 전시와 문화 프로그램\n모든 경험을 사진과 후기로 기록하세요.\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>해운대구의 매력을 느끼며 관광을 시작하세요.\n[해운대 블루라인파크](https://www.bluelinepark.com/)에서 스카이캡슐 또는 해변열차를 예약하세요.\n해변 구간을 달리며 옛 해안 절경을 감상하고, 위치 인증샷을 남기세요.\n탑승 중 또는 도착지에서 찍은 멋진 풍경 사진과 체험 후기를 기록하세요.\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>해운대구를 거닐며 여행 분위기를 즐기세요.\n[부산 요트투어 예약 링크](https://search.shopping.naver.com/search/all?query=%ED%95%B4%EC%9A%B4%EB%8C%80%20%EC%9A%94%ED%8A%B8%20%ED%88%AC%EC%96%B4&amp;frm=NVSCPRO&amp;nl-ts-pid=j4AErdqo1awsshZRDwGssssst1V-348234&amp;bt=-1)를 통해 원하는 시간과 코스를 선택하세요.\n요트에 승선해 바다 위에서의 특별한 순간을 즐기고 인증샷을 남기세요.\n바다 풍경과 함께 담은 인생샷과 체험 후기를 작성하세요.\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>해운대구 명소를 둘러보며 영화 관람 계획을 세우세요.\n2호선 센텀시티역 12번 출구에서 하차해 영화의전당으로 이동하세요.\n[영화의전당 예매 페이지](https://mobile.dureraum.org:44500/bccm/main/main.do?rbsIdx=1)에서 원하는 영화를 예약하거나, 더 라이브러리에서 무료 영화를 감상하세요.\n영화 관람 후 건물 외관이나 야경을 배경으로 인증샷을 찍고 후기를 남기세요.\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>금정구 일대를 둘러보며 문학과 역사 여행을 준비하세요.\n[요산 김정한 문학관](https://sayosan.or.kr/)을 찾아가 입구에서 첫 인증샷을 남기세요.\n김정한 작가의 생애와 작품 세계를 전시 자료와 함께 감상하세요.\n기억에 남는 전시물이나 글귀를 사진과 후기 형식으로 기록하세요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>금정구의 대표 사찰인 범어사를 목적지로 정하세요.\n범어사 일주문을 지나 경내로 걸어 들어가며 고즈넉한 분위기를 느껴보세요.\n대웅전, 범종각 등 주요 건물 앞에서 인증샷을 남기세요.\n사찰의 풍경과 느낀 점을 후기에 담아 기록하세요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>금정산 자락에 위치한 금정산성 코스를 계획하세요.\n등산로 또는 탐방로를 따라 금정산성에 도착하세요.\n산성의 성문, 성벽 등 역사적인 포인트에서 인증샷을 남기세요.\n산성과 금정구 전경을 함께 담은 사진과 함께 소감을 적어보세요.\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>금정구 속의 자연 명소인 회동수원지로 이동하세요.\n수변 산책로를 따라 걸으며 시원한 바람과 풍경을 즐기세요.\n물가나 나무 데크 구간에서 인증샷을 남기세요.\n고요한 분위기와 아름다운 자연을 후기에 기록하세요.\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>동래구를 거닐며 옛 부산의 역사와 문화를 느껴보세요.\n동래읍성 입구나 주요 성문(북문, 남문 등)에서 위치 인증샷을 찍으세요.\n성벽을 따라 걸으며 조선 시대 방어 시설과 주변 경관을 감상하세요.\n역사적인 배경과 함께 느낀 점을 후기에 기록하세요.\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>온천천을 따라 이어진 카페거리를 걸으며 여유로운 시간을 보내세요.\n강변 산책로에서 계절별 풍경을 배경으로 인증샷을 남기세요.\n마음에 드는 카페에 들러 음료를 즐기고 사진을 찍으세요.\n온천천과 카페거리의 매력을 후기에 담으세요.\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>동래구의 전통 온천 문화를 체험할 계획을 세우세요.\n온천탕이나 스파 시설에 방문해 위치 인증샷을 남기세요.\n따뜻한 온천물에 몸을 담그며 피로를 풀어보세요.\n온천 후 상쾌해진 기분과 추천 포인트를 후기에 작성하세요.\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>금강공원 입구로 이동해 케이블카 탑승 준비를 하세요.\n케이블카 승강장에서 위치 인증샷을 찍으세요.\n케이블카를 타고 금정산과 부산 시내 전망을 감상하세요.\n정상에서 바라본 경치와 케이블카 경험을 후기에 기록하세요.\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>중구로 이동해 독립·예술 영화의 매력을 느껴보세요.\nBNK부산은행 아트시네마 또는 모퉁이극장 입구에서 위치 인증샷을 찍으세요.\n상영작을 관람하며 영화 속 몰입감을 즐기세요.\n영화 감상 후 인상 깊었던 장면과 분위기를 후기에 기록하세요.\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>보수동 골목길로 들어서며 중구의 문화 향기를 느껴보세요.\n오래된 헌책방 간판과 골목 풍경을 배경으로 위치 인증샷을 남기세요.\n마음에 드는 책을 한 권 골라 구입하거나 읽어보세요.\n책방골목에서 느낀 레트로 감성과 발견한 책 이야기를 후기에 작성하세요.\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대청동 일대에 위치한 전망대로 이동하세요.\n전망대 입구나 내부에서 위치 인증샷을 남기세요.\n부산항과 남포동 일대가 한눈에 보이는 전망을 감상하세요.\n탁 트인 경치와 촬영한 사진을 후기에 기록하세요.\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아미동 골목길을 따라 비석마을로 향하세요.\n마을 입구나 벽화 앞에서 위치 인증샷을 찍으세요.\n독특한 역사와 사연이 깃든 마을을 천천히 걸으며 둘러보세요.\n마을의 분위기와 인상 깊었던 포인트를 후기에 남기세요.\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>중구 광복동에 있는 부산근현대역사관으로 이동하세요.\n역사관 입구에서 위치 인증샷을 남기세요.\n전시실을 둘러보며 부산의 근현대사를 배우세요.\n인상 깊었던 전시 내용과 느낀 점을 후기에 성하세요.\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>용두산공원으로 이동해 부산타워로 향하세요.\n타워 입구나 전망대에서 위치 인증샷을 남기세요.\n부산 시내 전경과 바다를 한눈에 내려다보며 감상하세요.\n찍은 사진과 함께 전망대에서의 경험을 후기에 남기세요.\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>동구로 이동해 창비부산 서점·문화공간을 방문하세요.\n입구 간판이나 내부 전경에서 위치 인증샷을 남기세요.\n책을 둘러보고, 마음에 드는 책을 골라 읽거나 구입하세요.\n책과 함께한 시간, 공간 분위기를 후기에 기록하세요.\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>초량이바구길 시작 지점으로 이동하세요.\n초량전망대나 벽화 앞에서 위치 인증샷을 찍으세요.\n길을 따라 부산항과 시내 전경을 감상하며 걸어보세요.\n산책 중 인상 깊었던 포인트와 사진을 후기에 남기세요.\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부산역 인근 차이나타운 입구로 이동하세요.\n붉은 아치형 간판이나 랜드마크 앞에서 위치 인증샷을 남기세요.\n중국풍 음식점, 상점, 거리 예술을 구경하며 즐기세요.\n먹은 음식과 거리 풍경 사진을 후기에 작성하세요.\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>168계단 인근에 위치한 야외영화관으로 이동하세요.\n영화관 전경 또는 좌석에서 위치 인증샷을 남기세요.\n야외에서 상영되는 영화를 감상하세요.\n관람한 영화와 야외 분위기를 후기에 남기세요.\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>한복 문화관으로 이동해 전통 의상을 체험하세요.\n입구 또는 한복 착용 후 위치 인증샷을 찍으세요.\n전통 의상과 소품을 활용해 사진 촬영을 즐기세요.\n체험 후 느낀 소감과 사진을 후기에 기록하세요.\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기장군 해안 절벽 위의 해동용궁사로 이동하세요.\n사찰 입구나 해안 풍경 앞에서 위치 인증샷을 남기세요.\n사찰 내부와 주변 경관을 둘러보며 사진 촬영하세요.\n해안 절경과 사찰의 매력을 후기에 작성하세요\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>테마파크 입구로 이동하세요.\n롯데월드 조형물 앞에서 위치 인증샷을 남기세요.\n놀이기구, 퍼레이드, 공연 등을 즐기세요.\n가장 즐거웠던 순간과 사진을 후기에 기록하세요.\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>루지 체험장 입구로 이동하세요.\n헬멧 착용 후 시작 지점에서 위치 인증샷을 남기세요.\n루지 트랙을 내려가며 짜릿한 속도를 즐기세요.\n체험 후 소감과 함께 사진을 후기에 남기세요.\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>연화리 해녀촌으로 이동하세요.\n해녀촌 간판이나 바다 풍경 앞에서 위치 인증샷을 남기세요.\n싱싱한 해산물 요리를 맛보세요.\n맛본 음식과 바닷가 풍경을 후기에 작성하세요.\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아홉산숲 입구로 이동하세요.\n숲길 표지판이나 대나무 숲 앞에서 위치 인증샷을 남기세요.\n대나무숲과 산책로를 따라 걸으며 자연을 느껴보세요.\n숲에서의 힐링 경험과 사진을 후기에 기록하세요.\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사하구 감천문화마을 입구로 이동하세요.\n마을 입구 조형물이나 지도 앞에서 위치 인증샷을 남기세요.\n골목길을 걸으며 벽화, 설치미술, 전망 포인트를 둘러보세요.\n가장 마음에 드는 작품이나 풍경을 사진과 함께 후기에 기록하세요.\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사하구 낙동강 하구에 위치한 부산현대미술관으로 이동하세요.\n미술관 전경이나 전시 안내판 앞에서 위치 인증샷을 남기세요.\n현재 진행 중인 전시를 관람하며 작품을 감상하세요.\n인상 깊었던 작품과 느낀 점을 후기에 작성하세요.\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>을숙도 생태공원 입구로 이동하세요.\n공원 표지판이나 전망대에서 위치 인증샷을 남기세요.\n습지, 갈대밭, 철새 서식지를 둘러보며 산책하세요.\n관찰한 풍경과 자연 속 경험을 후기에 기록하세요.\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>다대포해수욕장으로 이동하세요.\n해변 안내판이나 백사장 앞에서 위치 인증샷을 남기세요.\n바닷가를 산책하거나 노을 감상을 즐기세요.\n노을 사진과 해변에서의 추억을 후기에 남기세요.\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="3"/>
+      </rPr>
+      <t>사상구에</t>
     </r>
     <r>
       <rPr>
@@ -1656,7 +2146,7 @@
         <rFont val="Malgun Gothic"/>
         <family val="3"/>
       </rPr>
-      <t>사상구에</t>
+      <t>도착해</t>
     </r>
     <r>
       <rPr>
@@ -1676,7 +2166,7 @@
         <rFont val="Malgun Gothic"/>
         <family val="3"/>
       </rPr>
-      <t>도착해</t>
+      <t>삼락생태공원으로</t>
     </r>
     <r>
       <rPr>
@@ -1696,7 +2186,27 @@
         <rFont val="Malgun Gothic"/>
         <family val="3"/>
       </rPr>
-      <t>삼락생태공원으로</t>
+      <t>이동하세요</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.\n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="3"/>
+      </rPr>
+      <t>넓은</t>
     </r>
     <r>
       <rPr>
@@ -1716,7 +2226,127 @@
         <rFont val="Malgun Gothic"/>
         <family val="3"/>
       </rPr>
-      <t>이동하세요</t>
+      <t>잔디밭과</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="3"/>
+      </rPr>
+      <t>강변</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="3"/>
+      </rPr>
+      <t>산책로를</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="3"/>
+      </rPr>
+      <t>걸으며</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="3"/>
+      </rPr>
+      <t>여유로운</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="3"/>
+      </rPr>
+      <t>시간을</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="3"/>
+      </rPr>
+      <t>보내세요</t>
     </r>
     <r>
       <rPr>
@@ -1733,10 +2363,10 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Segoe UI Emoji"/>
-        <family val="2"/>
-      </rPr>
-      <t>2️⃣</t>
+        <rFont val="Malgun Gothic"/>
+        <family val="3"/>
+      </rPr>
+      <t>자전거</t>
     </r>
     <r>
       <rPr>
@@ -1756,7 +2386,7 @@
         <rFont val="Malgun Gothic"/>
         <family val="3"/>
       </rPr>
-      <t>넓은</t>
+      <t>대여소를</t>
     </r>
     <r>
       <rPr>
@@ -1776,7 +2406,7 @@
         <rFont val="Malgun Gothic"/>
         <family val="3"/>
       </rPr>
-      <t>잔디밭과</t>
+      <t>이용해</t>
     </r>
     <r>
       <rPr>
@@ -1816,7 +2446,7 @@
         <rFont val="Malgun Gothic"/>
         <family val="3"/>
       </rPr>
-      <t>산책로를</t>
+      <t>라이딩을</t>
     </r>
     <r>
       <rPr>
@@ -1836,7 +2466,27 @@
         <rFont val="Malgun Gothic"/>
         <family val="3"/>
       </rPr>
-      <t>걸으며</t>
+      <t>즐겨보세요</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.\n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="3"/>
+      </rPr>
+      <t>공원</t>
     </r>
     <r>
       <rPr>
@@ -1856,7 +2506,7 @@
         <rFont val="Malgun Gothic"/>
         <family val="3"/>
       </rPr>
-      <t>여유로운</t>
+      <t>전경을</t>
     </r>
     <r>
       <rPr>
@@ -1876,7 +2526,7 @@
         <rFont val="Malgun Gothic"/>
         <family val="3"/>
       </rPr>
-      <t>시간을</t>
+      <t>배경으로</t>
     </r>
     <r>
       <rPr>
@@ -1896,7 +2546,87 @@
         <rFont val="Malgun Gothic"/>
         <family val="3"/>
       </rPr>
-      <t>보내세요</t>
+      <t>인증샷을</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="3"/>
+      </rPr>
+      <t>남기고</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="3"/>
+      </rPr>
+      <t>체험</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="3"/>
+      </rPr>
+      <t>후기를</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="3"/>
+      </rPr>
+      <t>기록하세요</t>
     </r>
     <r>
       <rPr>
@@ -1909,1230 +2639,102 @@
       </rPr>
       <t>.\n</t>
     </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI Emoji"/>
-        <family val="2"/>
-      </rPr>
-      <t>3️⃣</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Malgun Gothic"/>
-        <family val="3"/>
-      </rPr>
-      <t>자전거</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Malgun Gothic"/>
-        <family val="3"/>
-      </rPr>
-      <t>대여소를</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Malgun Gothic"/>
-        <family val="3"/>
-      </rPr>
-      <t>이용해</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Malgun Gothic"/>
-        <family val="3"/>
-      </rPr>
-      <t>강변</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Malgun Gothic"/>
-        <family val="3"/>
-      </rPr>
-      <t>라이딩을</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Malgun Gothic"/>
-        <family val="3"/>
-      </rPr>
-      <t>즐겨보세요</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.\n</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI Emoji"/>
-        <family val="2"/>
-      </rPr>
-      <t>4️⃣</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Malgun Gothic"/>
-        <family val="3"/>
-      </rPr>
-      <t>공원</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Malgun Gothic"/>
-        <family val="3"/>
-      </rPr>
-      <t>전경을</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Malgun Gothic"/>
-        <family val="3"/>
-      </rPr>
-      <t>배경으로</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Malgun Gothic"/>
-        <family val="3"/>
-      </rPr>
-      <t>인증샷을</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Malgun Gothic"/>
-        <family val="3"/>
-      </rPr>
-      <t>남기고</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Malgun Gothic"/>
-        <family val="3"/>
-      </rPr>
-      <t>체험</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Malgun Gothic"/>
-        <family val="3"/>
-      </rPr>
-      <t>후기를</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Malgun Gothic"/>
-        <family val="3"/>
-      </rPr>
-      <t>기록하세요</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.\n</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://www.visitbusan.net/uploadImgs/files/cntnts/20230602100722403</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI Emoji"/>
-        <family val="2"/>
-      </rPr>
-      <t>🏺</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 사상생활사박물관 관람</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>옛 사상 지역의 생활과 역사를 엿볼 수 있는 공간</t>
-  </si>
-  <si>
-    <t>1️⃣ 사상생활사박물관으로 이동해 관람 준비를 하세요.\n2️⃣ 박물관 입구에서 방문 인증샷을 남기세요.\n3️⃣ 전시품과 생활사 자료를 꼼꼼히 둘러보세요.\n4️⃣ 인상 깊었던 전시를 사진과 후기로 기록하세요.\n</t>
-  </si>
-  <si>
-    <t>https://www.busan.go.kr/ImagePrint.do?dir=smartEditor&amp;savename=71426cee1ce844d4a9a54895f4457666&amp;realname=IMG_8531.JPG&amp;fileext=jpg&amp;filetype=image/jpeg&amp;filesize=125431</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>영도구</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI Emoji"/>
-        <family val="2"/>
-      </rPr>
-      <t>🪂</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 태종대 집라인 체험</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>바다 절벽 위 짜릿한 레저 스포츠</t>
-  </si>
-  <si>
-    <t>1️⃣ 영도구 태종대로 이동해 집라인 탑승 준비를 하세요.\n2️⃣ 안전장비를 착용 후 체험을 시작하세요.\n3️⃣ 탑승 전·후 태종대 절경을 배경으로 인증샷을 남기세요.\n4️⃣ 짜릿했던 순간을 사진과 후기로 남기세요.\n</t>
-  </si>
-  <si>
-    <t>https://www.visitbusan.net/uploadImgs/files/cntnts/20240718110728540</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI Symbol"/>
-        <family val="2"/>
-      </rPr>
-      <t>🏘</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 흰여울문화마을 산책</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>바다와 맞닿은 흰 담장 골목 예술마을</t>
-  </si>
-  <si>
-    <t>1️⃣ 영도 흰여울문화마을로 이동해 골목길을 따라 걸어보세요.\n2️⃣ 벽화, 갤러리, 바닷가 풍경을 감상하세요.\n3️⃣ 전망대에서 바다와 마을을 배경으로 인증샷을 남기세요.\n4️⃣ 감성적인 순간을 사진과 후기로 기록하세요.\n</t>
-  </si>
-  <si>
-    <t>https://www.agoda.com/wp-content/uploads/2024/08/Huinnyeoul-Culture-Village-Busan-featured-1244x700.jpg</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI Symbol"/>
-        <family val="2"/>
-      </rPr>
-      <t>🖼</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 아르떼뮤지엄 부산 탐방</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>몰입형 미디어아트 전시관</t>
-  </si>
-  <si>
-    <t>1️⃣ 영도구에 위치한 아르떼뮤지엄 부산으로 이동하세요.\n2️⃣ [아르떼뮤지엄 예매 페이지](https://artemuseum.com/)에서 티켓을 예매하세요.\n3️⃣ 입구에서 인증샷을 남기세요.\n4️⃣ 전시관 내부의 몰입형 작품을 감상하고 후기를 작성하세요.\n</t>
-  </si>
-  <si>
-    <t>https://www.visitbusan.net/uploadImgs/files/cntnts/20240912162614628_oen</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>강서구</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI Emoji"/>
-        <family val="2"/>
-      </rPr>
-      <t>🌿</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 맥도생태공원 산책</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>도심 속 습지와 철새를 만날 수 있는 생태공원</t>
-  </si>
-  <si>
-    <t>1️⃣ 강서구 맥도생태공원으로 이동하세요.\n2️⃣ 탐방로를 걸으며 철새와 습지 생태계를 감상하세요.\n3️⃣ 전망대에서 인증샷을 남기세요.\n4️⃣ 자연 속 힐링 경험을 사진과 후기로 기록하세요.\n</t>
-  </si>
-  <si>
-    <t>https://media.triple.guide/triple-cms/c_limit,f_auto,h_1024,w_1024/94526eee-db87-4a21-86be-fa8f037db618.jpeg</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>부산진구</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI Emoji"/>
-        <family val="2"/>
-      </rPr>
-      <t>🌳</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 부산시민공원 산책</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>도심 속에서 즐기는 여유로운 녹지 공간</t>
-  </si>
-  <si>
-    <t>1️⃣ 부산진구 부산시민공원으로 이동하세요.\n2️⃣ 산책로를 걸으며 다양한 조형물과 자연을 감상하세요.\n3️⃣ 공원 전경을 배경으로 인증샷을 남기세요.\n4️⃣ 힐링의 순간을 사진과 후기로 남기세요.\n</t>
-  </si>
-  <si>
-    <t>https://www.visitbusan.net/uploadImgs/files/cntnts/20191227194943122_oen</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI Emoji"/>
-        <family val="2"/>
-      </rPr>
-      <t>☕</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 전포 카페거리 투어</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>감각적인 카페와 맛집이 모인 핫플레이스</t>
-  </si>
-  <si>
-    <t>1️⃣ 부산진구 전포동 카페거리로 이동하세요.\n2️⃣ 개성 있는 카페와 매장을 탐방하세요.\n3️⃣ 카페 앞에서 인증샷을 남기세요.\n4️⃣ 맛있게 즐긴 메뉴와 분위기를 사진과 후기로 기록하세요.\n</t>
-  </si>
-  <si>
-    <t>https://www.visitbusan.net/uploadImgs/files/cntnts/20191227195612923</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI Emoji"/>
-        <family val="2"/>
-      </rPr>
-      <t>🌄</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 황령산 봉수대 전망</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>부산 야경을 한눈에 즐기는 명소</t>
-  </si>
-  <si>
-    <t>1️⃣ 황령산 봉수대로 이동해 산책을 즐기세요.\n2️⃣ 정상에서 부산 도심과 광안대교 전망을 감상하세요.\n3️⃣ 전망대에서 인증샷을 남기세요.\n4️⃣ 멋진 야경을 사진과 후기로 남기세요.\n</t>
-  </si>
-  <si>
-    <t>https://mblogthumb-phinf.pstatic.net/MjAyMDAyMTNfMTAg/MDAxNTgxNTYwNjQ3NDcx.Qx1iMfelSbQjsjrwHRiSir-5cYl6twb3YLaWSMd2kdQg.KfALGkJ_wnbuqg4L1JEzclP7L6hRY_qJlDY7Sr78W0Mg.JPEG.springlll8/1.JPG?type=w800</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI Emoji"/>
-        <family val="2"/>
-      </rPr>
-      <t>🎶</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 국립부산국악원 관람</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>우리 소리를 만나는 국악 전용 공연장</t>
-  </si>
-  <si>
-    <t>1️⃣ 부산진구 국립부산국악원으로 이동하세요.\n2️⃣ [공식 홈페이지](https://busan.gugak.go.kr/)에서 공연 일정을 확인하세요.\n3️⃣ 공연장 입구에서 인증샷을 남기세요.\n4️⃣ 전통 공연 감상 후 후기를 기록하세요.\n</t>
-  </si>
-  <si>
-    <t>https://www.visitbusan.net/uploadImgs/files/cntnts/20240822173844772_oen</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI Emoji"/>
-        <family val="2"/>
-      </rPr>
-      <t>🛕</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 삼광사 탐방</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>화려한 연등으로 유명한 사찰</t>
-  </si>
-  <si>
-    <t>1️⃣ 부산진구 삼광사로 이동하세요.\n2️⃣ 사찰 전경을 둘러보고 연등이 가득한 풍경을 감상하세요.\n3️⃣ 삼광사 정문이나 연등 거리에서 인증샷을 남기세요.\n4️⃣ 불교 문화 체험 소감을 후기로 작성하세요.\n</t>
-  </si>
-  <si>
-    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcTOwlmY8_U_7f1NUP_n3MGoJiqYq5X8ZrFLPg&amp;s</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI Symbol"/>
-        <family val="2"/>
-      </rPr>
-      <t>🛍</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 부전시장 탐방</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>부산 대표 전통시장 중 하나</t>
-  </si>
-  <si>
-    <t>1️⃣ 부산진구 부전시장으로 이동하세요.\n2️⃣ 다양한 먹거리와 상점을 둘러보세요.\n3️⃣ 시장 골목에서 인증샷을 남기세요.\n4️⃣ 맛있게 즐긴 음식과 시장 분위기를 후기로 기록하세요.\n</t>
-  </si>
-  <si>
-    <t>https://www.visitbusan.net/uploadImgs/files/cntnts/20191227113458027_oen</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>서구</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI Symbol"/>
-        <family val="2"/>
-      </rPr>
-      <t>🏖</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 송도해수욕장 즐기기</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>대한민국 최초의 해수욕장</t>
-  </si>
-  <si>
-    <t>1️⃣ 서구 송도해수욕장으로 이동하세요.\n2️⃣ 해변 산책로와 바다를 즐기세요.\n3️⃣ 송도 구름산책로에서 인증샷을 남기세요.\n4️⃣ 해수욕장의 추억을 사진과 후기로 기록하세요.\n</t>
-  </si>
-  <si>
-    <t>https://www.visitbusan.net/uploadImgs/files/cntnts/20191225175459392</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI Emoji"/>
-        <family val="2"/>
-      </rPr>
-      <t>🚡</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 송도해상케이블카 탑승</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>송도 바다 위를 나는 케이블카</t>
-  </si>
-  <si>
-    <t>1️⃣ 서구 송도해수욕장으로 이동해 케이블카 탑승장을 찾으세요.\n2️⃣ [송도 케이블카 예매 페이지](https://www.busanaircruise.co.kr/)에서 티켓을 예약하세요.\n3️⃣ 케이블카 안에서 바다 전망을 배경으로 인증샷을 남기세요.\n4️⃣ 멋진 풍경과 후기를 기록하세요.\n</t>
-  </si>
-  <si>
-    <t>https://www.visitbusan.net/uploadImgs/files/cntnts/20230508183214812</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI Emoji"/>
-        <family val="2"/>
-      </rPr>
-      <t>🎨</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 아미 비석문화마을 산책</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>예술과 역사가 공존하는 벽화 마을</t>
-  </si>
-  <si>
-    <t>1️⃣ 서구 아미동 비석마을로 이동하세요.\n2️⃣ 골목 곳곳에 남겨진 비석과 벽화를 감상하세요.\n3️⃣ 전망대에서 인증샷을 남기세요.\n4️⃣ 마을에서 느낀 감성을 사진과 후기로 기록하세요.\n</t>
-  </si>
-  <si>
-    <t>https://www.visitbusan.net/uploadImgs/files/cntnts/20191226093556574_oen</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI Emoji"/>
-        <family val="2"/>
-      </rPr>
-      <t>🌲</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 암남공원 탐방</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>천혜의 자연을 간직한 도심 속 공원</t>
-  </si>
-  <si>
-    <t>1️⃣ 서구 암남공원으로 이동하세요.\n2️⃣ 해안 산책로를 걸으며 자연 경관을 감상하세요.\n3️⃣ 전망대에서 인증샷을 남기세요.\n4️⃣ 힐링의 순간을 사진과 후기로 남기세요.\n</t>
-  </si>
-  <si>
-    <t>https://www.visitbusan.net/uploadImgs/files/cntnts/20191227112720208_oen</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI Symbol"/>
-        <family val="2"/>
-      </rPr>
-      <t>🏛</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 임시수도기념관 관람</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>한국전쟁 당시 임시수도의 역사를 담은 공간</t>
-  </si>
-  <si>
-    <t>1️⃣ 서구 임시수도기념관으로 이동하세요.\n2️⃣ 기념관 입구에서 인증샷을 남기세요.\n3️⃣ 전시실에서 한국전쟁과 부산의 역사 자료를 관람하세요.\n4️⃣ 기억에 남은 전시를 후기로 작성하세요.\n</t>
-  </si>
-  <si>
-    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcTyyao3EwU852Gs2a3-fpH2mu4D74a8WhliGQ&amp;s</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>남구</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI Symbol"/>
-        <family val="2"/>
-      </rPr>
-      <t>🕊</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 유엔평화기념관 방문</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>전쟁과 평화를 기억하는 국제적 공간</t>
-  </si>
-  <si>
-    <t>1️⃣ 남구 대연동 UN기념공원으로 이동하세요.\n2️⃣ 묘역과 평화공원을 걸으며 참배하세요.\n3️⃣ UN평화기념관에서 인증샷을 남기세요.\n4️⃣ 평화의 의미를 되새기며 후기를 기록하세요.\n</t>
-  </si>
-  <si>
-    <t>https://mblogthumb-phinf.pstatic.net/MjAyNDA3MjRfNTMg/MDAxNzIxODAxMTE3Mjg4.Lw9UAUpgllbjysF742wVLtx8qtjExbd2MGsFIDfBCbgg.2o8cJbl0EEKd5qSaam1laNOSRbnyfoAoLFr2S1Hlb90g.JPEG/%EC%82%AC%EC%A7%846.jpg?type=w800</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI Emoji"/>
-        <family val="2"/>
-      </rPr>
-      <t>🏺</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 부산박물관 관람</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>부산의 역사와 문화를 한눈에 볼 수 있는 곳</t>
-  </si>
-  <si>
-    <t>1️⃣ 남구 부산박물관으로 이동하세요.\n2️⃣ [부산박물관 홈페이지](https://museum.busan.go.kr/)에서 전시 일정을 확인하세요.\n3️⃣ 박물관 입구에서 인증샷을 남기세요.\n4️⃣ 인상 깊었던 전시를 사진과 후기로 기록하세요.\n</t>
-  </si>
-  <si>
-    <t>https://museum.busan.go.kr/humanframe/theme/museum_busan_2025/assets/img/content/exhibitorigin0001.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI Emoji"/>
-        <family val="2"/>
-      </rPr>
-      <t>🌊</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 이기대 해안산책</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>해안 절경과 트레킹 코스를 즐길 수 있는 명소</t>
-  </si>
-  <si>
-    <t>1️⃣ 남구 이기대로 이동하세요.\n2️⃣ 해안산책로를 따라 걷거나 트레킹을 즐기세요.\n3️⃣ 전망대에서 광안대교와 바다를 배경으로 인증샷을 남기세요.\n4️⃣ 아름다운 풍경을 사진과 후기로 기록하세요.\n</t>
-  </si>
-  <si>
-    <t>https://i.namu.wiki/i/pLygk_uCGnTjhllty4djNljfJWcAqwt9zi-bIl4AE_xfZe764Z0D9iSw9aYWuauMlSxOQxuptAecnvEDoLB1wg.webp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>북구</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI Emoji"/>
-        <family val="2"/>
-      </rPr>
-      <t>🌿</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 화명생태공원 탐방</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>강과 숲이 어우러진 생태체험 공간</t>
-  </si>
-  <si>
-    <t>1️⃣ 북구 화명생태공원으로 이동하세요.\n2️⃣ 강변 산책로를 걸으며 생태계를 감상하세요.\n3️⃣ 공원 내 포토존에서 인증샷을 남기세요.\n4️⃣ 자연 체험 소감을 후기로 기록하세요.\n</t>
-  </si>
-  <si>
-    <t>https://localsegye.co.kr/news/data/2025/03/07/p1065569622910044_923_thum.JPG</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI Emoji"/>
-        <family val="2"/>
-      </rPr>
-      <t>🌹</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 화명장미공원 감상</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>화려한 장미가 만개하는 힐링 명소</t>
-  </si>
-  <si>
-    <t>1️⃣ 북구 장미원으로 이동하세요.\n2️⃣ 계절별 장미꽃이 핀 정원을 감상하세요.\n3️⃣ 만개한 장미 앞에서 인증샷을 남기세요.\n4️⃣ 꽃향기 가득한 추억을 후기로 기록하세요.\n</t>
-  </si>
-  <si>
-    <t>https://www.visitbusan.net/uploadImgs/files/cntnts/20230519190619574</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI Symbol"/>
-        <family val="2"/>
-      </rPr>
-      <t>🛍</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 구포시장 탐방</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>북구 대표 전통시장</t>
-  </si>
-  <si>
-    <t>1️⃣ 북구 구포시장으로 이동하세요.\n2️⃣ 시장 골목을 걸으며 다양한 먹거리를 즐기세요.\n3️⃣ 시장 입구에서 인증샷을 남기세요.\n4️⃣ 시장 분위기와 맛본 음식을 후기로 기록하세요.\n</t>
-  </si>
-  <si>
-    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcTCIlXoYpHO16msUWEyjdmN_ZWyda2HjNpurH6EPX5IaPHe7MWaF7scT2u5JzHJwZ3Vr5w&amp;usqp=CAU</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>연제구</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI Emoji"/>
-        <family val="2"/>
-      </rPr>
-      <t>🛕</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 마하사 탐방</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>연제구의 고즈넉한 사찰</t>
-  </si>
-  <si>
-    <t>1️⃣ 연제구 마하사로 이동하세요.\n2️⃣ 사찰 전경을 둘러보고 경내를 산책하세요.\n3️⃣ 대웅전 앞에서 인증샷을 남기세요.\n4️⃣ 사찰에서 느낀 평온한 분위기를 후기로 기록하세요.\n</t>
-  </si>
-  <si>
-    <t>https://www.visitbusan.net/uploadImgs/files/cntnts/20240911101725976</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI Emoji"/>
-        <family val="2"/>
-      </rPr>
-      <t>🏺</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 연산동 고분군 관람</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>가야시대 고분 유적지 탐방</t>
-  </si>
-  <si>
-    <t>1️⃣ 연제구 연산동 고분군으로 이동하세요.\n2️⃣ 고분군 안내판과 유적을 둘러보세요.\n3️⃣ 유적지 전경을 배경으로 인증샷을 남기세요.\n4️⃣ 역사 탐방 소감을 후기로 기록하세요.\n</t>
-  </si>
-  <si>
-    <t>https://i.namu.wiki/i/ehwWOBrnbUCrjhJJ2Qsyukxmr6NppuZqVAYlyLrgAKhIiYhRiHthdO28IY7m6DXms6CmzF_h7lK-UDbFleJpxw.webp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Apple Color Emoji"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>1️⃣</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 금정구 속의 자연 명소인 회동수원지로 이동하세요.\n</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Apple Color Emoji"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>2️⃣</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 수변 산책로를 따라 걸으며 시원한 바람과 풍경을 즐기세요.\n</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Apple Color Emoji"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>3️⃣</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 물가나 나무 데크 구간에서 인증샷을 남기세요.\n</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Apple Color Emoji"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>4️⃣</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 고요한 분위기와 아름다운 자연을 후기에 기록하세요.\n</t>
-    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사상생활사박물관으로 이동해 관람 준비를 하세요.\n박물관 입구에서 방문 인증샷을 남기세요.\n전시품과 생활사 자료를 꼼꼼히 둘러보세요.\n인상 깊었던 전시를 사진과 후기로 기록하세요.\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영도구 태종대로 이동해 집라인 탑승 준비를 하세요.\n안전장비를 착용 후 체험을 시작하세요.\n탑승 전·후 태종대 절경을 배경으로 인증샷을 남기세요.\n짜릿했던 순간을 사진과 후기로 남기세요.\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영도 흰여울문화마을로 이동해 골목길을 따라 걸어보세요.\n벽화, 갤러리, 바닷가 풍경을 감상하세요.\n전망대에서 바다와 마을을 배경으로 인증샷을 남기세요.\n감성적인 순간을 사진과 후기로 기록하세요.\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영도구에 위치한 아르떼뮤지엄 부산으로 이동하세요.\n[아르떼뮤지엄 예매 페이지](https://artemuseum.com/)에서 티켓을 예매하세요.\n입구에서 인증샷을 남기세요.\n전시관 내부의 몰입형 작품을 감상하고 후기를 작성하세요.\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>강서구 맥도생태공원으로 이동하세요.\n탐방로를 걸으며 철새와 습지 생태계를 감상하세요.\n전망대에서 인증샷을 남기세요.\n자연 속 힐링 경험을 사진과 후기로 기록하세요.\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부산진구 부산시민공원으로 이동하세요.\n산책로를 걸으며 다양한 조형물과 자연을 감상하세요.\n공원 전경을 배경으로 인증샷을 남기세요.\n힐링의 순간을 사진과 후기로 남기세요.\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부산진구 전포동 카페거리로 이동하세요.\n개성 있는 카페와 매장을 탐방하세요.\n카페 앞에서 인증샷을 남기세요.\n맛있게 즐긴 메뉴와 분위기를 사진과 후기로 기록하세요.\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>황령산 봉수대로 이동해 산책을 즐기세요.\n정상에서 부산 도심과 광안대교 전망을 감상하세요.\n전망대에서 인증샷을 남기세요.\n멋진 야경을 사진과 후기로 남기세요.\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부산진구 국립부산국악원으로 이동하세요.\n[공식 홈페이지](https://busan.gugak.go.kr/)에서 공연 일정을 확인하세요.\n공연장 입구에서 인증샷을 남기세요.\n전통 공연 감상 후 후기를 기록하세요.\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부산진구 삼광사로 이동하세요.\n사찰 전경을 둘러보고 연등이 가득한 풍경을 감상하세요.\n삼광사 정문이나 연등 거리에서 인증샷을 남기세요.\n불교 문화 체험 소감을 후기로 작성하세요.\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부산진구 부전시장으로 이동하세요.\n다양한 먹거리와 상점을 둘러보세요.\n시장 골목에서 인증샷을 남기세요.\n맛있게 즐긴 음식과 시장 분위기를 후기로 기록하세요.\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서구 송도해수욕장으로 이동하세요.\n해변 산책로와 바다를 즐기세요.\n송도 구름산책로에서 인증샷을 남기세요.\n해수욕장의 추억을 사진과 후기로 기록하세요.\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서구 송도해수욕장으로 이동해 케이블카 탑승장을 찾으세요.\n[송도 케이블카 예매 페이지](https://www.busanaircruise.co.kr/)에서 티켓을 예약하세요.\n케이블카 안에서 바다 전망을 배경으로 인증샷을 남기세요.\n멋진 풍경과 후기를 기록하세요.\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서구 아미동 비석마을로 이동하세요.\n골목 곳곳에 남겨진 비석과 벽화를 감상하세요.\n전망대에서 인증샷을 남기세요.\n마을에서 느낀 감성을 사진과 후기로 기록하세요.\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서구 암남공원으로 이동하세요.\n해안 산책로를 걸으며 자연 경관을 감상하세요.\n전망대에서 인증샷을 남기세요.\n힐링의 순간을 사진과 후기로 남기세요.\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서구 임시수도기념관으로 이동하세요.\n기념관 입구에서 인증샷을 남기세요.\n전시실에서 한국전쟁과 부산의 역사 자료를 관람하세요.\n기억에 남은 전시를 후기로 작성하세요.\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>남구 대연동 UN기념공원으로 이동하세요.\n묘역과 평화공원을 걸으며 참배하세요.\nUN평화기념관에서 인증샷을 남기세요.\n평화의 의미를 되새기며 후기를 기록하세요.\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>남구 부산박물관으로 이동하세요.\n[부산박물관 홈페이지](https://museum.busan.go.kr/)에서 전시 일정을 확인하세요.\n박물관 입구에서 인증샷을 남기세요.\n인상 깊었던 전시를 사진과 후기로 기록하세요.\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>남구 이기대로 이동하세요.\n해안산책로를 따라 걷거나 트레킹을 즐기세요.\n전망대에서 광안대교와 바다를 배경으로 인증샷을 남기세요.\n아름다운 풍경을 사진과 후기로 기록하세요.\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>북구 화명생태공원으로 이동하세요.\n강변 산책로를 걸으며 생태계를 감상하세요.\n공원 내 포토존에서 인증샷을 남기세요.\n자연 체험 소감을 후기로 기록하세요.\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>북구 장미원으로 이동하세요.\n계절별 장미꽃이 핀 정원을 감상하세요.\n만개한 장미 앞에서 인증샷을 남기세요.\n꽃향기 가득한 추억을 후기로 기록하세요.\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>북구 구포시장으로 이동하세요.\n시장 골목을 걸으며 다양한 먹거리를 즐기세요.\n시장 입구에서 인증샷을 남기세요.\n시장 분위기와 맛본 음식을 후기로 기록하세요.\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>연제구 마하사로 이동하세요.\n사찰 전경을 둘러보고 경내를 산책하세요.\n대웅전 앞에서 인증샷을 남기세요.\n사찰에서 느낀 평온한 분위기를 후기로 기록하세요.\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>연제구 연산동 고분군으로 이동하세요.\n고분군 안내판과 유적을 둘러보세요.\n유적지 전경을 배경으로 인증샷을 남기세요.\n역사 탐방 소감을 후기로 기록하세요.\n</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3639,7 +3241,7 @@
     <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="55" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="topRight" activeCell="B3" sqref="B3"/>
+      <selection pane="topRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="18"/>
@@ -3687,7 +3289,7 @@
         <v>18</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>120</v>
+        <v>203</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>119</v>
@@ -3699,7 +3301,7 @@
         <v>35.162999999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="76">
+    <row r="3" spans="1:7" ht="82">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -3710,7 +3312,7 @@
         <v>19</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>121</v>
+        <v>204</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>53</v>
@@ -3733,7 +3335,7 @@
         <v>20</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>122</v>
+        <v>205</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>54</v>
@@ -3756,7 +3358,7 @@
         <v>21</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>123</v>
+        <v>206</v>
       </c>
       <c r="E5" t="s">
         <v>55</v>
@@ -3779,7 +3381,7 @@
         <v>22</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>124</v>
+        <v>207</v>
       </c>
       <c r="E6" t="s">
         <v>56</v>
@@ -3802,7 +3404,7 @@
         <v>23</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>125</v>
+        <v>208</v>
       </c>
       <c r="E7" t="s">
         <v>57</v>
@@ -3825,7 +3427,7 @@
         <v>24</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>126</v>
+        <v>209</v>
       </c>
       <c r="E8" t="s">
         <v>58</v>
@@ -3837,7 +3439,7 @@
         <v>35.171391999999997</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="57">
+    <row r="9" spans="1:7" ht="38">
       <c r="A9" s="4" t="s">
         <v>10</v>
       </c>
@@ -3848,7 +3450,7 @@
         <v>25</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>127</v>
+        <v>210</v>
       </c>
       <c r="E9" t="s">
         <v>59</v>
@@ -3871,7 +3473,7 @@
         <v>26</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>128</v>
+        <v>211</v>
       </c>
       <c r="E10" t="s">
         <v>60</v>
@@ -3894,7 +3496,7 @@
         <v>27</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>129</v>
+        <v>212</v>
       </c>
       <c r="E11" t="s">
         <v>61</v>
@@ -3906,7 +3508,7 @@
         <v>35.277479</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="50">
+    <row r="12" spans="1:7" ht="38">
       <c r="A12" s="4" t="s">
         <v>10</v>
       </c>
@@ -3917,7 +3519,7 @@
         <v>28</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>262</v>
+        <v>213</v>
       </c>
       <c r="E12" t="s">
         <v>62</v>
@@ -3940,7 +3542,7 @@
         <v>29</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>130</v>
+        <v>214</v>
       </c>
       <c r="E13" t="s">
         <v>63</v>
@@ -3963,7 +3565,7 @@
         <v>30</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>131</v>
+        <v>215</v>
       </c>
       <c r="E14" t="s">
         <v>64</v>
@@ -3986,7 +3588,7 @@
         <v>31</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>132</v>
+        <v>216</v>
       </c>
       <c r="E15" t="s">
         <v>65</v>
@@ -4009,7 +3611,7 @@
         <v>32</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>133</v>
+        <v>217</v>
       </c>
       <c r="E16" t="s">
         <v>66</v>
@@ -4032,7 +3634,7 @@
         <v>33</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>134</v>
+        <v>218</v>
       </c>
       <c r="E17" t="s">
         <v>67</v>
@@ -4055,7 +3657,7 @@
         <v>34</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>135</v>
+        <v>219</v>
       </c>
       <c r="E18" t="s">
         <v>68</v>
@@ -4078,7 +3680,7 @@
         <v>35</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>136</v>
+        <v>220</v>
       </c>
       <c r="E19" t="s">
         <v>69</v>
@@ -4101,7 +3703,7 @@
         <v>36</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>137</v>
+        <v>221</v>
       </c>
       <c r="E20" t="s">
         <v>70</v>
@@ -4124,7 +3726,7 @@
         <v>37</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>138</v>
+        <v>222</v>
       </c>
       <c r="E21" t="s">
         <v>71</v>
@@ -4147,7 +3749,7 @@
         <v>38</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>139</v>
+        <v>223</v>
       </c>
       <c r="E22" t="s">
         <v>72</v>
@@ -4170,7 +3772,7 @@
         <v>39</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>140</v>
+        <v>224</v>
       </c>
       <c r="E23" t="s">
         <v>73</v>
@@ -4193,7 +3795,7 @@
         <v>40</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>141</v>
+        <v>225</v>
       </c>
       <c r="E24" t="s">
         <v>74</v>
@@ -4216,7 +3818,7 @@
         <v>41</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>142</v>
+        <v>226</v>
       </c>
       <c r="E25" t="s">
         <v>75</v>
@@ -4239,7 +3841,7 @@
         <v>42</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>143</v>
+        <v>227</v>
       </c>
       <c r="E26" t="s">
         <v>76</v>
@@ -4262,7 +3864,7 @@
         <v>43</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>144</v>
+        <v>228</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>77</v>
@@ -4285,7 +3887,7 @@
         <v>44</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>145</v>
+        <v>229</v>
       </c>
       <c r="E28" t="s">
         <v>78</v>
@@ -4308,7 +3910,7 @@
         <v>45</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>146</v>
+        <v>230</v>
       </c>
       <c r="E29" t="s">
         <v>79</v>
@@ -4331,7 +3933,7 @@
         <v>46</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>147</v>
+        <v>231</v>
       </c>
       <c r="E30" t="s">
         <v>80</v>
@@ -4354,7 +3956,7 @@
         <v>47</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>81</v>
@@ -4377,7 +3979,7 @@
         <v>48</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>149</v>
+        <v>233</v>
       </c>
       <c r="E32" t="s">
         <v>82</v>
@@ -4400,7 +4002,7 @@
         <v>49</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>150</v>
+        <v>234</v>
       </c>
       <c r="E33" t="s">
         <v>83</v>
@@ -4423,7 +4025,7 @@
         <v>50</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>151</v>
+        <v>235</v>
       </c>
       <c r="E34" t="s">
         <v>84</v>
@@ -4446,7 +4048,7 @@
         <v>51</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>152</v>
+        <v>236</v>
       </c>
       <c r="E35" t="s">
         <v>85</v>
@@ -4469,7 +4071,7 @@
         <v>52</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>153</v>
+        <v>237</v>
       </c>
       <c r="E36" t="s">
         <v>86</v>
@@ -4483,19 +4085,19 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="4" t="s">
-        <v>154</v>
+        <v>120</v>
       </c>
       <c r="B37" t="s">
-        <v>155</v>
+        <v>121</v>
       </c>
       <c r="C37" t="s">
-        <v>156</v>
-      </c>
-      <c r="D37" t="s">
-        <v>157</v>
+        <v>122</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>238</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>158</v>
+        <v>123</v>
       </c>
       <c r="F37" s="5">
         <v>128.97337899999999</v>
@@ -4506,19 +4108,19 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="4" t="s">
-        <v>154</v>
+        <v>120</v>
       </c>
       <c r="B38" t="s">
-        <v>159</v>
+        <v>124</v>
       </c>
       <c r="C38" t="s">
-        <v>160</v>
+        <v>125</v>
       </c>
       <c r="D38" t="s">
-        <v>161</v>
+        <v>239</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>162</v>
+        <v>126</v>
       </c>
       <c r="F38" s="5">
         <v>128.97888800000001</v>
@@ -4529,19 +4131,19 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="4" t="s">
-        <v>163</v>
+        <v>127</v>
       </c>
       <c r="B39" t="s">
-        <v>164</v>
+        <v>128</v>
       </c>
       <c r="C39" t="s">
-        <v>165</v>
+        <v>129</v>
       </c>
       <c r="D39" t="s">
-        <v>166</v>
+        <v>240</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>167</v>
+        <v>130</v>
       </c>
       <c r="F39" s="5">
         <v>129.072396</v>
@@ -4552,19 +4154,19 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="4" t="s">
-        <v>163</v>
+        <v>127</v>
       </c>
       <c r="B40" t="s">
-        <v>168</v>
+        <v>131</v>
       </c>
       <c r="C40" t="s">
-        <v>169</v>
+        <v>132</v>
       </c>
       <c r="D40" t="s">
-        <v>170</v>
+        <v>241</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>171</v>
+        <v>133</v>
       </c>
       <c r="F40" s="5">
         <v>129.04520600000001</v>
@@ -4575,19 +4177,19 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="4" t="s">
-        <v>163</v>
+        <v>127</v>
       </c>
       <c r="B41" t="s">
-        <v>172</v>
+        <v>134</v>
       </c>
       <c r="C41" t="s">
-        <v>173</v>
+        <v>135</v>
       </c>
       <c r="D41" t="s">
-        <v>174</v>
+        <v>242</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>175</v>
+        <v>136</v>
       </c>
       <c r="F41" s="5">
         <v>129.042586</v>
@@ -4598,19 +4200,19 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="4" t="s">
-        <v>176</v>
+        <v>137</v>
       </c>
       <c r="B42" t="s">
-        <v>177</v>
+        <v>138</v>
       </c>
       <c r="C42" t="s">
-        <v>178</v>
+        <v>139</v>
       </c>
       <c r="D42" t="s">
-        <v>179</v>
+        <v>243</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>180</v>
+        <v>140</v>
       </c>
       <c r="F42" s="5">
         <v>128.95568499999999</v>
@@ -4621,19 +4223,19 @@
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="4" t="s">
-        <v>181</v>
+        <v>141</v>
       </c>
       <c r="B43" t="s">
-        <v>182</v>
+        <v>142</v>
       </c>
       <c r="C43" t="s">
-        <v>183</v>
+        <v>143</v>
       </c>
       <c r="D43" t="s">
-        <v>184</v>
+        <v>244</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>185</v>
+        <v>144</v>
       </c>
       <c r="F43" s="5">
         <v>129.05749700000001</v>
@@ -4644,19 +4246,19 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="4" t="s">
-        <v>181</v>
+        <v>141</v>
       </c>
       <c r="B44" t="s">
-        <v>186</v>
+        <v>145</v>
       </c>
       <c r="C44" t="s">
-        <v>187</v>
+        <v>146</v>
       </c>
       <c r="D44" t="s">
-        <v>188</v>
+        <v>245</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>189</v>
+        <v>147</v>
       </c>
       <c r="F44" s="5">
         <v>129.066543</v>
@@ -4667,19 +4269,19 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="4" t="s">
-        <v>181</v>
+        <v>141</v>
       </c>
       <c r="B45" t="s">
-        <v>190</v>
+        <v>148</v>
       </c>
       <c r="C45" t="s">
-        <v>191</v>
+        <v>149</v>
       </c>
       <c r="D45" t="s">
-        <v>192</v>
+        <v>246</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>193</v>
+        <v>150</v>
       </c>
       <c r="F45" s="5">
         <v>129.082716</v>
@@ -4690,19 +4292,19 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="4" t="s">
-        <v>181</v>
+        <v>141</v>
       </c>
       <c r="B46" t="s">
-        <v>194</v>
+        <v>151</v>
       </c>
       <c r="C46" t="s">
-        <v>195</v>
+        <v>152</v>
       </c>
       <c r="D46" t="s">
-        <v>196</v>
+        <v>247</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>197</v>
+        <v>153</v>
       </c>
       <c r="F46" s="5">
         <v>129.05429100000001</v>
@@ -4713,19 +4315,19 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="4" t="s">
-        <v>181</v>
+        <v>141</v>
       </c>
       <c r="B47" t="s">
-        <v>198</v>
+        <v>154</v>
       </c>
       <c r="C47" t="s">
-        <v>199</v>
+        <v>155</v>
       </c>
       <c r="D47" t="s">
-        <v>200</v>
+        <v>248</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>201</v>
+        <v>156</v>
       </c>
       <c r="F47" s="5">
         <v>129.04353699999999</v>
@@ -4736,19 +4338,19 @@
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="4" t="s">
-        <v>181</v>
+        <v>141</v>
       </c>
       <c r="B48" t="s">
-        <v>202</v>
+        <v>157</v>
       </c>
       <c r="C48" t="s">
-        <v>203</v>
+        <v>158</v>
       </c>
       <c r="D48" t="s">
-        <v>204</v>
+        <v>249</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>205</v>
+        <v>159</v>
       </c>
       <c r="F48" s="5">
         <v>129.06128100000001</v>
@@ -4759,19 +4361,19 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="4" t="s">
-        <v>206</v>
+        <v>160</v>
       </c>
       <c r="B49" t="s">
-        <v>207</v>
+        <v>161</v>
       </c>
       <c r="C49" t="s">
-        <v>208</v>
+        <v>162</v>
       </c>
       <c r="D49" t="s">
-        <v>209</v>
+        <v>250</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>210</v>
+        <v>163</v>
       </c>
       <c r="F49" s="5">
         <v>129.016997</v>
@@ -4782,19 +4384,19 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="4" t="s">
-        <v>206</v>
+        <v>160</v>
       </c>
       <c r="B50" t="s">
-        <v>211</v>
+        <v>164</v>
       </c>
       <c r="C50" t="s">
-        <v>212</v>
+        <v>165</v>
       </c>
       <c r="D50" t="s">
-        <v>213</v>
+        <v>251</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>214</v>
+        <v>166</v>
       </c>
       <c r="F50" s="5">
         <v>129.02014500000001</v>
@@ -4805,19 +4407,19 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="4" t="s">
-        <v>206</v>
+        <v>160</v>
       </c>
       <c r="B51" t="s">
-        <v>215</v>
+        <v>167</v>
       </c>
       <c r="C51" t="s">
-        <v>216</v>
+        <v>168</v>
       </c>
       <c r="D51" t="s">
-        <v>217</v>
+        <v>252</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>218</v>
+        <v>169</v>
       </c>
       <c r="F51" s="5">
         <v>129.01319799999999</v>
@@ -4828,19 +4430,19 @@
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="4" t="s">
-        <v>206</v>
+        <v>160</v>
       </c>
       <c r="B52" t="s">
-        <v>219</v>
+        <v>170</v>
       </c>
       <c r="C52" t="s">
-        <v>220</v>
+        <v>171</v>
       </c>
       <c r="D52" t="s">
-        <v>221</v>
+        <v>253</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>222</v>
+        <v>172</v>
       </c>
       <c r="F52" s="5">
         <v>129.016246</v>
@@ -4851,19 +4453,19 @@
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="4" t="s">
-        <v>206</v>
+        <v>160</v>
       </c>
       <c r="B53" t="s">
-        <v>223</v>
+        <v>173</v>
       </c>
       <c r="C53" t="s">
-        <v>224</v>
+        <v>174</v>
       </c>
       <c r="D53" t="s">
-        <v>225</v>
+        <v>254</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>226</v>
+        <v>175</v>
       </c>
       <c r="F53" s="5">
         <v>129.01776000000001</v>
@@ -4874,19 +4476,19 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="4" t="s">
-        <v>227</v>
+        <v>176</v>
       </c>
       <c r="B54" t="s">
-        <v>228</v>
+        <v>177</v>
       </c>
       <c r="C54" t="s">
-        <v>229</v>
+        <v>178</v>
       </c>
       <c r="D54" t="s">
-        <v>230</v>
+        <v>255</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>231</v>
+        <v>179</v>
       </c>
       <c r="F54" s="5">
         <v>129.09299899999999</v>
@@ -4897,19 +4499,19 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="4" t="s">
-        <v>227</v>
+        <v>176</v>
       </c>
       <c r="B55" t="s">
-        <v>232</v>
+        <v>180</v>
       </c>
       <c r="C55" t="s">
-        <v>233</v>
+        <v>181</v>
       </c>
       <c r="D55" t="s">
-        <v>234</v>
+        <v>256</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>235</v>
+        <v>182</v>
       </c>
       <c r="F55" s="5">
         <v>129.09324000000001</v>
@@ -4920,19 +4522,19 @@
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="4" t="s">
-        <v>227</v>
+        <v>176</v>
       </c>
       <c r="B56" t="s">
-        <v>236</v>
+        <v>183</v>
       </c>
       <c r="C56" t="s">
-        <v>237</v>
+        <v>184</v>
       </c>
       <c r="D56" t="s">
-        <v>238</v>
+        <v>257</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>239</v>
+        <v>185</v>
       </c>
       <c r="F56" s="5">
         <v>129.121273</v>
@@ -4943,19 +4545,19 @@
     </row>
     <row r="57" spans="1:7">
       <c r="A57" s="4" t="s">
-        <v>240</v>
+        <v>186</v>
       </c>
       <c r="B57" t="s">
-        <v>241</v>
+        <v>187</v>
       </c>
       <c r="C57" t="s">
-        <v>242</v>
+        <v>188</v>
       </c>
       <c r="D57" t="s">
-        <v>243</v>
+        <v>258</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>244</v>
+        <v>189</v>
       </c>
       <c r="F57" s="5">
         <v>129.00695999999999</v>
@@ -4966,19 +4568,19 @@
     </row>
     <row r="58" spans="1:7">
       <c r="A58" s="4" t="s">
-        <v>240</v>
+        <v>186</v>
       </c>
       <c r="B58" t="s">
-        <v>245</v>
+        <v>190</v>
       </c>
       <c r="C58" t="s">
-        <v>246</v>
+        <v>191</v>
       </c>
       <c r="D58" t="s">
-        <v>247</v>
+        <v>259</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>248</v>
+        <v>192</v>
       </c>
       <c r="F58" s="5">
         <v>129.010222</v>
@@ -4989,19 +4591,19 @@
     </row>
     <row r="59" spans="1:7">
       <c r="A59" s="7" t="s">
-        <v>240</v>
+        <v>186</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>249</v>
+        <v>193</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>250</v>
+        <v>194</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>251</v>
+        <v>260</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>252</v>
+        <v>195</v>
       </c>
       <c r="F59" s="5">
         <v>129.004155</v>
@@ -5012,19 +4614,19 @@
     </row>
     <row r="60" spans="1:7">
       <c r="A60" s="4" t="s">
-        <v>253</v>
+        <v>196</v>
       </c>
       <c r="B60" t="s">
-        <v>254</v>
+        <v>197</v>
       </c>
       <c r="C60" t="s">
-        <v>255</v>
+        <v>198</v>
       </c>
       <c r="D60" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>257</v>
+        <v>199</v>
       </c>
       <c r="F60" s="5">
         <v>129.08894900000001</v>
@@ -5035,19 +4637,19 @@
     </row>
     <row r="61" spans="1:7">
       <c r="A61" s="4" t="s">
-        <v>253</v>
+        <v>196</v>
       </c>
       <c r="B61" t="s">
-        <v>258</v>
+        <v>200</v>
       </c>
       <c r="C61" t="s">
-        <v>259</v>
+        <v>201</v>
       </c>
       <c r="D61" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>261</v>
+        <v>202</v>
       </c>
       <c r="F61" s="5">
         <v>129.09171599999999</v>

</xml_diff>